<commit_message>
Remove SBtab_ from the name inside the excel files
</commit_message>
<xml_diff>
--- a/SBTAB_Viswan_2018.xlsx
+++ b/SBTAB_Viswan_2018.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santos\Documents\Git\Thesis_Code\Subcellular_Workflow_Matlab\Model\Model_Findsim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santos\Documents\Git\Thesis_Code\Subcellular_Workflow_Matlab\Model\Model_Viswan_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93128651-5003-4CCB-A0F7-4BCBE1307224}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E0AD5A-5F47-4E22-8C5D-0E4EB635D641}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21196" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5370" yWindow="2220" windowWidth="28800" windowHeight="15472" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defaults" sheetId="13" r:id="rId1"/>
@@ -3668,40 +3668,40 @@
     <t>Time_E1T0_Y1</t>
   </si>
   <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Viswan_2018' TableName='Experiments' TableTitle='SBTAB_Viswan_2018 Experiments' TableType = 'QuantityMatrix'</t>
-  </si>
-  <si>
-    <t>TableName='Defaults' TableType='Quantity' TableTitle='Default units for this model' SBtabVersion='1.0' Document='SBTAB_Viswan_2018'</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Viswan_2018' TableName='Compartment' TableTitle='SBTAB_Viswan_2018 Compound' TableType = 'Quantity'</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Viswan_2018' TableName='Compound' TableTitle='SBTAB_Viswan_2018 Compound' TableType = 'Compound'</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Viswan_2018' TableName='Parameter' TableTitle='SBTAB_Viswan_2018 Parameter' TableType = 'Quantity'</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Viswan_2018' TableName='Reaction' TableTitle='SBTAB_Viswan_2018 Reaction' TableType = 'Reaction'</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Viswan_2018' TableName='Output' TableTitle='SBTAB_Viswan_2018 Output' TableType = 'Quantity'</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Viswan_2018' TableName='Expression' TableTitle='SBTAB_Viswan_2018 Expression' TableType = 'Expression'</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Viswan_2018' TableName='E0' TableTitle='SBTAB_Viswan_2018 E0' TableType = 'QuantityMatrix'</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Viswan_2018' TableName='E0I' TableTitle='SBTAB_Viswan_2018 E0I' TableType = 'QuantityMatrix'</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Viswan_2018' TableName='E1' TableTitle='SBTAB_Viswan_2018 E1' TableType = 'QuantityMatrix'</t>
-  </si>
-  <si>
-    <t>SBtabVersion='1.0' Document='SBTAB_Viswan_2018' TableName='E1I' TableTitle='SBTAB_Viswan_2018 E1I' TableType = 'QuantityMatrix'</t>
+    <t>SBtabVersion='1.0' Document='Viswan_2018' TableName='Compartment' TableTitle='Viswan_2018 Compound' TableType = 'Quantity'</t>
+  </si>
+  <si>
+    <t>TableName='Defaults' TableType='Quantity' TableTitle='Default units for this model' SBtabVersion='1.0' Document='Viswan_2018'</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='Viswan_2018' TableName='Compound' TableTitle='Viswan_2018 Compound' TableType = 'Compound'</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='Viswan_2018' TableName='Parameter' TableTitle='Viswan_2018 Parameter' TableType = 'Quantity'</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='Viswan_2018' TableName='Reaction' TableTitle='Viswan_2018 Reaction' TableType = 'Reaction'</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='Viswan_2018' TableName='Output' TableTitle='Viswan_2018 Output' TableType = 'Quantity'</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='Viswan_2018' TableName='Expression' TableTitle='Viswan_2018 Expression' TableType = 'Expression'</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='Viswan_2018' TableName='Experiments' TableTitle='Viswan_2018 Experiments' TableType = 'QuantityMatrix'</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='Viswan_2018' TableName='E0' TableTitle='Viswan_2018 E0' TableType = 'QuantityMatrix'</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='Viswan_2018' TableName='E0I' TableTitle='Viswan_2018 E0I' TableType = 'QuantityMatrix'</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='Viswan_2018' TableName='E1' TableTitle='Viswan_2018 E1' TableType = 'QuantityMatrix'</t>
+  </si>
+  <si>
+    <t>SBtabVersion='1.0' Document='Viswan_2018' TableName='E1I' TableTitle='Viswan_2018 E1I' TableType = 'QuantityMatrix'</t>
   </si>
 </sst>
 </file>
@@ -4388,7 +4388,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4403,7 +4403,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -4463,7 +4463,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -7794,7 +7794,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -13459,7 +13459,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -15964,7 +15964,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -16086,7 +16086,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -16148,7 +16148,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1208</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.45">

</xml_diff>